<commit_message>
Change columns names: [Start day]->[Start] and [End day]->[End]
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -69,10 +69,10 @@
     <t xml:space="preserve">5 tasks, no bounds</t>
   </si>
   <si>
-    <t xml:space="preserve">Start day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End day</t>
+    <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End</t>
   </si>
   <si>
     <t xml:space="preserve">Work</t>
@@ -315,7 +315,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -378,10 +378,6 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -573,7 +569,7 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -772,7 +768,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -780,7 +776,7 @@
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="16" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -819,16 +815,16 @@
       <c r="C2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="17" t="n">
+      <c r="D2" s="16" t="n">
         <v>45642</v>
       </c>
-      <c r="E2" s="17" t="n">
+      <c r="E2" s="16" t="n">
         <v>45840</v>
       </c>
-      <c r="F2" s="17" t="n">
+      <c r="F2" s="16" t="n">
         <v>45642</v>
       </c>
-      <c r="G2" s="17" t="n">
+      <c r="G2" s="16" t="n">
         <v>45840</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -854,7 +850,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1262,7 +1258,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1725,7 +1721,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2120,7 +2116,7 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2579,7 +2575,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2974,7 +2970,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3171,7 +3167,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Change form of input file: add images paramaters
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -20,6 +20,12 @@
     <sheet name="invoicing periods bounds" sheetId="10" state="visible" r:id="rId12"/>
     <sheet name="public holidays" sheetId="11" state="visible" r:id="rId13"/>
     <sheet name="misc" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="himg" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="timg" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="simg" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="gimg" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="wimg" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="bimg" sheetId="18" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -192,28 +198,112 @@
     <t xml:space="preserve">Hours per day</t>
   </si>
   <si>
-    <t xml:space="preserve">dpi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T:start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T:end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H:start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H:end</t>
-  </si>
-  <si>
     <t xml:space="preserve">Solver</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-12-15</t>
+    <t xml:space="preserve">Last day</t>
   </si>
   <si>
     <t xml:space="preserve">scip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dpi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar:color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar:hatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar:alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Start OK?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is End OK?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#2ca02c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasks per day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#d62728</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hours per day stacked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task's Gantt Chart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barh:color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barh:height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barh:alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#ff7f0e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoicing Periods Workload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar:ecolor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar:capsize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#7BC8F6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#EE0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task with bounds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill:color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill:hatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill:alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot:format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot:markeredgewidth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step:linewidth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#90EE90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o</t>
   </si>
 </sst>
 </file>
@@ -225,7 +315,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -260,8 +350,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,6 +375,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFD7"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD8CE"/>
+        <bgColor rgb="FFFFD7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A933"/>
+        <bgColor rgb="FF008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFFFD8CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -315,7 +436,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -380,7 +501,27 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -418,7 +559,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -434,7 +575,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFD8CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -444,7 +585,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -569,7 +710,7 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -648,7 +789,7 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -731,7 +872,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -766,17 +907,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -789,46 +930,562 @@
       <c r="C1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>59</v>
+      <c r="A2" s="12" t="n">
+        <v>45641</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="D2" s="16" t="n">
+      <c r="C2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="17" t="n">
+        <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C900))</f>
+        <v>45840</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="23.18"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="E2" s="20" t="n">
         <v>45642</v>
       </c>
-      <c r="E2" s="16" t="n">
+      <c r="F2" s="20" t="n">
         <v>45840</v>
       </c>
-      <c r="F2" s="16" t="n">
+      <c r="G2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J2" s="21" t="b">
+        <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="21" t="b">
+        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="E2" s="20" t="n">
         <v>45642</v>
       </c>
-      <c r="G2" s="16" t="n">
+      <c r="F2" s="20" t="n">
         <v>45840</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>60</v>
+      <c r="G2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J2" s="21" t="b">
+        <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="21" t="b">
+        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="E2" s="20" t="n">
+        <v>45642</v>
+      </c>
+      <c r="F2" s="20" t="n">
+        <v>45840</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H2" s="21" t="b">
+        <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="21" t="b">
+        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="E2" s="20" t="n">
+        <v>45642</v>
+      </c>
+      <c r="F2" s="20" t="n">
+        <v>45840</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J2" s="21" t="b">
+        <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="21" t="b">
+        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.91"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="4" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +1506,7 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1101,7 +1758,7 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1257,7 +1914,7 @@
   </sheetPr>
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1720,7 +2377,7 @@
   </sheetPr>
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2115,7 +2772,7 @@
   </sheetPr>
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2574,7 +3231,7 @@
   </sheetPr>
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2969,7 +3626,7 @@
   </sheetPr>
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3166,7 +3823,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change date range for [Hours pay day stacked] chart in Excel files
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -505,7 +505,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -909,7 +909,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1162,8 +1162,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,7 +1215,8 @@
         <v>45642</v>
       </c>
       <c r="F2" s="20" t="n">
-        <v>45840</v>
+        <f aca="false">E2+20</f>
+        <v>45662</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>0.6</v>

</xml_diff>

<commit_message>
Shorten horizon time for view data in examples
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -968,7 +968,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1027,7 +1027,8 @@
         <v>45642</v>
       </c>
       <c r="F2" s="20" t="n">
-        <v>45840</v>
+        <f aca="false">E2+20</f>
+        <v>45662</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>64</v>
@@ -1066,7 +1067,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1124,7 +1125,8 @@
         <v>45642</v>
       </c>
       <c r="F2" s="20" t="n">
-        <v>45840</v>
+        <f aca="false">E2+20</f>
+        <v>45662</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>67</v>
@@ -1162,8 +1164,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1248,7 +1250,7 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove input data Start, End form Gant chart
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="89">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -1248,16 +1248,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1274,25 +1274,13 @@
         <v>58</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,28 +1293,14 @@
       <c r="D2" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="20" t="n">
-        <v>45642</v>
-      </c>
-      <c r="F2" s="20" t="n">
-        <v>45840</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="F2" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="G2" s="4" t="n">
         <v>0.6</v>
-      </c>
-      <c r="J2" s="21" t="b">
-        <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
-        <v>1</v>
-      </c>
-      <c r="K2" s="21" t="b">
-        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add invoicing periods bounds to example 01
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -36,8 +36,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid expert?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valid period?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="79">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -144,46 +180,16 @@
     <t xml:space="preserve">25.Jan</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-12-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-01-15</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.Feb</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-01-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-02-13</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.Mar</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-02-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-03-16</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.Apr</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-03-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-04-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">25.May</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-04-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-05-18</t>
   </si>
   <si>
     <t xml:space="preserve">Period</t>
@@ -379,14 +385,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <fgColor rgb="FFFFD8CE"/>
+        <bgColor rgb="FFFFD7D7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD8CE"/>
-        <bgColor rgb="FFFFD7D7"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -436,7 +442,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -489,23 +495,43 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -513,12 +539,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -711,7 +733,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -787,17 +809,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="13" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="14" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -805,7 +829,7 @@
         <v>30</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>32</v>
@@ -813,31 +837,124 @@
       <c r="D1" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="E1" s="16" t="b">
+        <f aca="false">AND(E2:E832)</f>
+        <v>1</v>
+      </c>
+      <c r="F1" s="16" t="b">
+        <f aca="false">AND(F2:F832)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E2" s="18" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$921, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="18" t="b">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B2) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E3" s="18" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$921, A3) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="18" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B3) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E4" s="18" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$921, A4) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="18" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B4) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E5" s="18" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$921, A5) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="18" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B5) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E6" s="18" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$921, A6) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="18" t="n">
+        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B6) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
@@ -862,6 +979,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -883,7 +1001,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,16 +1040,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>54</v>
+        <v>43</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,9 +1060,9 @@
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="17" t="n">
+        <v>45</v>
+      </c>
+      <c r="D2" s="22" t="n">
         <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C900))</f>
         <v>45840</v>
       </c>
@@ -979,17 +1097,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>52</v>
+      <c r="A1" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>12</v>
@@ -998,19 +1116,19 @@
         <v>13</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,27 +1141,27 @@
       <c r="D2" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="20" t="n">
+      <c r="E2" s="19" t="n">
         <v>45642</v>
       </c>
-      <c r="F2" s="20" t="n">
+      <c r="F2" s="19" t="n">
         <f aca="false">E2+20</f>
         <v>45662</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="J2" s="21" t="b">
+      <c r="J2" s="25" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="21" t="b">
+      <c r="K2" s="25" t="b">
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
         <v>1</v>
       </c>
@@ -1077,17 +1195,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>66</v>
+      <c r="A1" s="23" t="s">
+        <v>56</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>12</v>
@@ -1096,19 +1214,19 @@
         <v>13</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1121,27 +1239,27 @@
       <c r="D2" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="20" t="n">
+      <c r="E2" s="19" t="n">
         <v>45642</v>
       </c>
-      <c r="F2" s="20" t="n">
+      <c r="F2" s="19" t="n">
         <f aca="false">E2+20</f>
         <v>45662</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="J2" s="21" t="b">
+      <c r="J2" s="25" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="21" t="b">
+      <c r="K2" s="25" t="b">
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
         <v>1</v>
       </c>
@@ -1175,17 +1293,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>69</v>
+      <c r="A1" s="23" t="s">
+        <v>59</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>12</v>
@@ -1194,13 +1312,13 @@
         <v>13</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,21 +1331,21 @@
       <c r="D2" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="20" t="n">
+      <c r="E2" s="19" t="n">
         <v>45642</v>
       </c>
-      <c r="F2" s="20" t="n">
+      <c r="F2" s="19" t="n">
         <f aca="false">E2+20</f>
         <v>45662</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>0.6</v>
       </c>
-      <c r="H2" s="21" t="b">
+      <c r="H2" s="25" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="21" t="b">
+      <c r="I2" s="25" t="b">
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
         <v>1</v>
       </c>
@@ -1250,7 +1368,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -1261,26 +1379,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>70</v>
+      <c r="A1" s="23" t="s">
+        <v>60</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,7 +1412,7 @@
         <v>150</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>0.9</v>
@@ -1332,26 +1450,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>75</v>
+      <c r="A1" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1365,10 +1483,10 @@
         <v>150</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>4</v>
@@ -1405,35 +1523,35 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>80</v>
+      <c r="A1" s="23" t="s">
+        <v>70</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,16 +1565,16 @@
         <v>150</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0.5</v>
@@ -3798,98 +3916,121 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="12" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="14" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="15" t="s">
         <v>13</v>
       </c>
+      <c r="D1" s="16" t="b">
+        <f aca="false">AND(D2:D908)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="n">
+        <v>45637</v>
+      </c>
+      <c r="C2" s="11" t="n">
+        <v>45672</v>
+      </c>
+      <c r="D2" s="18" t="b">
+        <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="B3" s="11" t="n">
+        <v>45673</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>45701</v>
+      </c>
+      <c r="D3" s="18" t="n">
+        <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="B4" s="11" t="n">
+        <v>45702</v>
+      </c>
+      <c r="C4" s="11" t="n">
+        <v>45732</v>
+      </c>
+      <c r="D4" s="18" t="n">
+        <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B5" s="11" t="n">
+        <v>45733</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>45761</v>
+      </c>
+      <c r="D5" s="18" t="n">
+        <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>48</v>
+      <c r="B6" s="11" t="n">
+        <v>45762</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>45795</v>
+      </c>
+      <c r="D6" s="18" t="n">
+        <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Create report [Experts per day stacked]
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,6 +26,7 @@
     <sheet name="gimg" sheetId="16" state="visible" r:id="rId18"/>
     <sheet name="wimg" sheetId="17" state="visible" r:id="rId19"/>
     <sheet name="bimg" sheetId="18" state="visible" r:id="rId20"/>
+    <sheet name="eimg" sheetId="19" state="visible" r:id="rId21"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -49,7 +50,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -62,7 +62,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid period?</t>
         </r>
@@ -73,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="80">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -310,6 +309,9 @@
   </si>
   <si>
     <t xml:space="preserve">o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experts per day stacked</t>
   </si>
 </sst>
 </file>
@@ -321,7 +323,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -355,6 +357,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -442,7 +449,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -495,11 +502,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -507,16 +510,12 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -535,7 +534,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -811,17 +810,17 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="4" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="13" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="14" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -837,11 +836,11 @@
       <c r="D1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="16" t="b">
+      <c r="E1" s="15" t="b">
         <f aca="false">AND(E2:E832)</f>
         <v>1</v>
       </c>
-      <c r="F1" s="16" t="b">
+      <c r="F1" s="15" t="b">
         <f aca="false">AND(F2:F832)</f>
         <v>1</v>
       </c>
@@ -850,7 +849,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -859,11 +858,11 @@
       <c r="D2" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E2" s="18" t="b">
+      <c r="E2" s="13" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$921, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F2" s="18" t="b">
+      <c r="F2" s="13" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B2) &gt; 0</f>
         <v>1</v>
       </c>
@@ -872,7 +871,7 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -881,11 +880,11 @@
       <c r="D3" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E3" s="18" t="n">
+      <c r="E3" s="13" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$921, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F3" s="18" t="n">
+      <c r="F3" s="13" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B3) &gt; 0</f>
         <v>1</v>
       </c>
@@ -894,7 +893,7 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -903,11 +902,11 @@
       <c r="D4" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E4" s="18" t="n">
+      <c r="E4" s="13" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$921, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F4" s="18" t="n">
+      <c r="F4" s="13" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B4) &gt; 0</f>
         <v>1</v>
       </c>
@@ -916,7 +915,7 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -925,11 +924,11 @@
       <c r="D5" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E5" s="18" t="n">
+      <c r="E5" s="13" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$921, A5) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F5" s="18" t="n">
+      <c r="F5" s="13" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B5) &gt; 0</f>
         <v>1</v>
       </c>
@@ -938,7 +937,7 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -947,29 +946,26 @@
       <c r="D6" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="E6" s="18" t="n">
+      <c r="E6" s="13" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$921, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F6" s="18" t="n">
+      <c r="F6" s="13" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B6) &gt; 0</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1048,7 +1044,7 @@
       <c r="C1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1062,7 +1058,7 @@
       <c r="C2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="22" t="n">
+      <c r="D2" s="20" t="n">
         <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C900))</f>
         <v>45840</v>
       </c>
@@ -1097,7 +1093,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1124,10 +1120,10 @@
       <c r="I1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1141,10 +1137,10 @@
       <c r="D2" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="19" t="n">
+      <c r="E2" s="17" t="n">
         <v>45642</v>
       </c>
-      <c r="F2" s="19" t="n">
+      <c r="F2" s="17" t="n">
         <f aca="false">E2+20</f>
         <v>45662</v>
       </c>
@@ -1157,11 +1153,11 @@
       <c r="I2" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="J2" s="25" t="b">
+      <c r="J2" s="23" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="25" t="b">
+      <c r="K2" s="23" t="b">
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
         <v>1</v>
       </c>
@@ -1195,7 +1191,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1222,10 +1218,10 @@
       <c r="I1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1239,10 +1235,10 @@
       <c r="D2" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="19" t="n">
+      <c r="E2" s="17" t="n">
         <v>45642</v>
       </c>
-      <c r="F2" s="19" t="n">
+      <c r="F2" s="17" t="n">
         <f aca="false">E2+20</f>
         <v>45662</v>
       </c>
@@ -1255,11 +1251,11 @@
       <c r="I2" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="J2" s="25" t="b">
+      <c r="J2" s="23" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="25" t="b">
+      <c r="K2" s="23" t="b">
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
         <v>1</v>
       </c>
@@ -1293,7 +1289,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1314,10 +1310,10 @@
       <c r="G1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1331,21 +1327,21 @@
       <c r="D2" s="4" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="19" t="n">
+      <c r="E2" s="17" t="n">
         <v>45642</v>
       </c>
-      <c r="F2" s="19" t="n">
+      <c r="F2" s="17" t="n">
         <f aca="false">E2+20</f>
         <v>45662</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>0.6</v>
       </c>
-      <c r="H2" s="25" t="b">
+      <c r="H2" s="23" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="25" t="b">
+      <c r="I2" s="23" t="b">
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
         <v>1</v>
       </c>
@@ -1379,7 +1375,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1450,7 +1446,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1523,7 +1519,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1581,6 +1577,65 @@
       </c>
       <c r="J2" s="4" t="n">
         <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>150</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -3927,26 +3982,26 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="12" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="14" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="16" t="b">
+      <c r="D1" s="15" t="b">
         <f aca="false">AND(D2:D908)</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="11" t="n">
@@ -3955,13 +4010,13 @@
       <c r="C2" s="11" t="n">
         <v>45672</v>
       </c>
-      <c r="D2" s="18" t="b">
+      <c r="D2" s="13" t="b">
         <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="11" t="n">
@@ -3970,13 +4025,13 @@
       <c r="C3" s="11" t="n">
         <v>45701</v>
       </c>
-      <c r="D3" s="18" t="n">
+      <c r="D3" s="13" t="b">
         <f aca="false">AND(ISNUMBER(B3), ISNUMBER(C3), B3&lt;=C3)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="11" t="n">
@@ -3985,13 +4040,13 @@
       <c r="C4" s="11" t="n">
         <v>45732</v>
       </c>
-      <c r="D4" s="18" t="n">
+      <c r="D4" s="13" t="b">
         <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="11" t="n">
@@ -4000,13 +4055,13 @@
       <c r="C5" s="11" t="n">
         <v>45761</v>
       </c>
-      <c r="D5" s="18" t="n">
+      <c r="D5" s="13" t="b">
         <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="11" t="n">
@@ -4015,22 +4070,22 @@
       <c r="C6" s="11" t="n">
         <v>45795</v>
       </c>
-      <c r="D6" s="18" t="n">
+      <c r="D6" s="13" t="b">
         <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Apply sparse model for AMPL
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,28 +5,26 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="tasks" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="links" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="task" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="assign" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="xbday" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="xbsum" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="ubday" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="ubsum" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="expert bounds" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="invoicing periods" sheetId="9" state="visible" r:id="rId11"/>
-    <sheet name="invoicing periods bounds" sheetId="10" state="visible" r:id="rId12"/>
-    <sheet name="public holidays" sheetId="11" state="visible" r:id="rId13"/>
-    <sheet name="misc" sheetId="12" state="visible" r:id="rId14"/>
-    <sheet name="himg" sheetId="13" state="visible" r:id="rId15"/>
-    <sheet name="timg" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="simg" sheetId="15" state="visible" r:id="rId17"/>
-    <sheet name="gimg" sheetId="16" state="visible" r:id="rId18"/>
-    <sheet name="wimg" sheetId="17" state="visible" r:id="rId19"/>
-    <sheet name="bimg" sheetId="18" state="visible" r:id="rId20"/>
-    <sheet name="eimg" sheetId="19" state="visible" r:id="rId21"/>
+    <sheet name="ubday" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="ebday" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="period" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="pbsum" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="holiday" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="misc" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="himg" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="timg" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="simg" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="gimg" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="wimg" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="bimg" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="eimg" sheetId="17" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -37,7 +35,7 @@
 </workbook>
 </file>
 
-<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author>Unknown Author</author>
@@ -72,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="80">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -808,219 +806,6 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="4" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="13" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="15" t="b">
-        <f aca="false">AND(E2:E832)</f>
-        <v>1</v>
-      </c>
-      <c r="F1" s="15" t="b">
-        <f aca="false">AND(F2:F832)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="E2" s="13" t="b">
-        <f aca="false">COUNTIF(experts!$A$2:$A$921, A2) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="13" t="b">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B2) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="E3" s="13" t="b">
-        <f aca="false">COUNTIF(experts!$A$2:$A$921, A3) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="13" t="b">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B3) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="E4" s="13" t="b">
-        <f aca="false">COUNTIF(experts!$A$2:$A$921, A4) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="13" t="b">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B4) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="E5" s="13" t="b">
-        <f aca="false">COUNTIF(experts!$A$2:$A$921, A5) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="13" t="b">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B5) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="E6" s="13" t="b">
-        <f aca="false">COUNTIF(experts!$A$2:$A$921, A6) &gt; 0</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="13" t="b">
-        <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B6) &gt; 0</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="n">
-        <v>45651</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1059,7 +844,7 @@
         <v>45</v>
       </c>
       <c r="D2" s="20" t="n">
-        <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C900))</f>
+        <f aca="false">MAX(MAX(period!C2:C900),MAX(task!C2:C900))</f>
         <v>45840</v>
       </c>
     </row>
@@ -1074,7 +859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1173,7 +958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1271,7 +1056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1357,7 +1142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1428,7 +1213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1499,7 +1284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1590,14 +1375,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2525,401 +2310,6 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F70"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="4" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -3374,402 +2764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F70"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="4" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3966,7 +2961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4096,4 +3091,217 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="13" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="15" t="b">
+        <f aca="false">AND(E2:E832)</f>
+        <v>1</v>
+      </c>
+      <c r="F1" s="15" t="b">
+        <f aca="false">AND(F2:F832)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E2" s="13" t="b">
+        <f aca="false">COUNTIF(expert!$A$2:$A$921, A2) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="13" t="b">
+        <f aca="false">COUNTIF(period!$A$2:$A$1000, B2) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E3" s="13" t="b">
+        <f aca="false">COUNTIF(expert!$A$2:$A$921, A3) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="13" t="b">
+        <f aca="false">COUNTIF(period!$A$2:$A$1000, B3) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E4" s="13" t="b">
+        <f aca="false">COUNTIF(expert!$A$2:$A$921, A4) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="13" t="b">
+        <f aca="false">COUNTIF(period!$A$2:$A$1000, B4) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E5" s="13" t="b">
+        <f aca="false">COUNTIF(expert!$A$2:$A$921, A5) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="13" t="b">
+        <f aca="false">COUNTIF(period!$A$2:$A$1000, B5) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E6" s="13" t="b">
+        <f aca="false">COUNTIF(expert!$A$2:$A$921, A6) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="13" t="b">
+        <f aca="false">COUNTIF(period!$A$2:$A$1000, B6) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="n">
+        <v>45651</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change names from *img to img*
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
@@ -18,13 +18,13 @@
     <sheet name="pbsum" sheetId="8" state="visible" r:id="rId10"/>
     <sheet name="holiday" sheetId="9" state="visible" r:id="rId11"/>
     <sheet name="misc" sheetId="10" state="visible" r:id="rId12"/>
-    <sheet name="himg" sheetId="11" state="visible" r:id="rId13"/>
-    <sheet name="timg" sheetId="12" state="visible" r:id="rId14"/>
-    <sheet name="simg" sheetId="13" state="visible" r:id="rId15"/>
-    <sheet name="gimg" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="wimg" sheetId="15" state="visible" r:id="rId17"/>
-    <sheet name="bimg" sheetId="16" state="visible" r:id="rId18"/>
-    <sheet name="eimg" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="imgh" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="imgt" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="imgs" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="imgg" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="imgw" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="imgb" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="imge" sheetId="17" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -1382,7 +1382,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -3276,7 +3276,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Extend the image [Invoid period workload]
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="80">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -1382,7 +1382,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2969,7 +2969,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3098,10 +3098,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3127,11 +3127,11 @@
         <v>33</v>
       </c>
       <c r="E1" s="15" t="b">
-        <f aca="false">AND(E2:E832)</f>
+        <f aca="false">AND(E2:E834)</f>
         <v>1</v>
       </c>
       <c r="F1" s="15" t="b">
-        <f aca="false">AND(F2:F832)</f>
+        <f aca="false">AND(F2:F834)</f>
         <v>1</v>
       </c>
     </row>
@@ -3159,16 +3159,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="E3" s="13" t="b">
         <f aca="false">COUNTIF(expert!$A$2:$A$921, A3) &gt; 0</f>
@@ -3181,16 +3181,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="E4" s="13" t="b">
         <f aca="false">COUNTIF(expert!$A$2:$A$921, A4) &gt; 0</f>
@@ -3203,7 +3203,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>34</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>34</v>
@@ -3245,17 +3245,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E7" s="13" t="b">
+        <f aca="false">COUNTIF(expert!$A$2:$A$921, A7) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="13" t="b">
+        <f aca="false">COUNTIF(period!$A$2:$A$1000, B7) &gt; 0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="E8" s="13" t="b">
+        <f aca="false">COUNTIF(expert!$A$2:$A$921, A8) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="13" t="b">
+        <f aca="false">COUNTIF(period!$A$2:$A$1000, B8) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
+    </row>
+    <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Add option [With UBDAY]
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="82">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -204,10 +204,16 @@
     <t xml:space="preserve">Solver</t>
   </si>
   <si>
+    <t xml:space="preserve">With ubday</t>
+  </si>
+  <si>
     <t xml:space="preserve">Last day</t>
   </si>
   <si>
     <t xml:space="preserve">scip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">Width</t>
@@ -730,7 +736,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D1:D2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -806,17 +812,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -829,8 +835,11 @@
       <c r="C1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="7" t="s">
         <v>44</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,9 +850,12 @@
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="20" t="n">
+        <v>46</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="20" t="n">
         <f aca="false">MAX(MAX(period!C2:C900),MAX(task!C2:C900))</f>
         <v>45840</v>
       </c>
@@ -867,7 +879,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="D1:D2 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -882,13 +894,13 @@
         <v>42</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>12</v>
@@ -897,19 +909,19 @@
         <v>13</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,10 +942,10 @@
         <v>45662</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0.3</v>
@@ -943,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="23" t="b">
-        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
+        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!E2)</f>
         <v>1</v>
       </c>
     </row>
@@ -966,7 +978,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="D1:D2 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -977,16 +989,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>12</v>
@@ -995,19 +1007,19 @@
         <v>13</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,10 +1040,10 @@
         <v>45662</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0.3</v>
@@ -1041,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="23" t="b">
-        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
+        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!E2)</f>
         <v>1</v>
       </c>
     </row>
@@ -1064,7 +1076,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="D1:D2 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1075,16 +1087,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>12</v>
@@ -1093,13 +1105,13 @@
         <v>13</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="23" t="b">
-        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
+        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!E2)</f>
         <v>1</v>
       </c>
     </row>
@@ -1150,7 +1162,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="D1:D2 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1161,25 +1173,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,7 +1205,7 @@
         <v>150</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>0.9</v>
@@ -1221,7 +1233,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1232,25 +1244,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,10 +1276,10 @@
         <v>150</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>4</v>
@@ -1292,7 +1304,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1305,34 +1317,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,16 +1358,16 @@
         <v>150</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0.5</v>
@@ -1383,7 +1395,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="D1:D2 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1394,19 +1406,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,7 +1454,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D2 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1694,7 +1706,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="D1:D2 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1850,7 +1862,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2313,7 +2325,7 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D2 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2772,7 +2784,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D2 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2969,7 +2981,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="D1:D2 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3100,8 +3112,8 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="1" sqref="D1:D2 F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3321,7 +3333,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D1:D2 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Create spreadsheet [img] and define one [start,end] date range
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
@@ -18,13 +18,14 @@
     <sheet name="pbsum" sheetId="8" state="visible" r:id="rId10"/>
     <sheet name="holiday" sheetId="9" state="visible" r:id="rId11"/>
     <sheet name="misc" sheetId="10" state="visible" r:id="rId12"/>
-    <sheet name="imgh" sheetId="11" state="visible" r:id="rId13"/>
-    <sheet name="imgt" sheetId="12" state="visible" r:id="rId14"/>
-    <sheet name="imgs" sheetId="13" state="visible" r:id="rId15"/>
-    <sheet name="imgg" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="imgw" sheetId="15" state="visible" r:id="rId17"/>
-    <sheet name="imgb" sheetId="16" state="visible" r:id="rId18"/>
-    <sheet name="imge" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="img" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="imgh" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="imgt" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="imgs" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="imgg" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="imgw" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="imgb" sheetId="17" state="visible" r:id="rId19"/>
+    <sheet name="imge" sheetId="18" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -216,6 +217,9 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
+    <t xml:space="preserve">For all charts</t>
+  </si>
+  <si>
     <t xml:space="preserve">Width</t>
   </si>
   <si>
@@ -225,6 +229,12 @@
     <t xml:space="preserve">Dpi</t>
   </si>
   <si>
+    <t xml:space="preserve">Is Start OK?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is End OK?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bar:color</t>
   </si>
   <si>
@@ -232,12 +242,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bar:alpha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is Start OK?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is End OK?</t>
   </si>
   <si>
     <t xml:space="preserve">#2ca02c</t>
@@ -375,7 +379,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,7 +401,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD8CE"/>
-        <bgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFFFFFD7"/>
       </patternFill>
     </fill>
     <fill>
@@ -410,12 +414,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00A933"/>
         <bgColor rgb="FF008000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD7D7"/>
-        <bgColor rgb="FFFFD8CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -453,7 +451,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -546,10 +544,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,7 +578,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFFFD7D7"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -736,7 +730,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D1:D2 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -814,8 +808,8 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -876,31 +870,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="D1:D2 F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="23.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>12</v>
@@ -908,53 +901,36 @@
       <c r="F1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="7" t="s">
+      <c r="G1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="H1" s="22" t="s">
         <v>53</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>150</v>
       </c>
       <c r="E2" s="17" t="n">
+        <f aca="false">misc!A2+1</f>
         <v>45642</v>
       </c>
       <c r="F2" s="17" t="n">
         <f aca="false">E2+20</f>
         <v>45662</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="J2" s="23" t="b">
+      <c r="G2" s="13" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="23" t="b">
+      <c r="H2" s="13" t="b">
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!E2)</f>
         <v>1</v>
       </c>
@@ -975,86 +951,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="D1:D2 F2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="23.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>4</v>
-      </c>
       <c r="D2" s="4" t="n">
-        <v>150</v>
-      </c>
-      <c r="E2" s="17" t="n">
-        <v>45642</v>
-      </c>
-      <c r="F2" s="17" t="n">
-        <f aca="false">E2+20</f>
-        <v>45662</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="I2" s="4" t="n">
         <v>0.3</v>
-      </c>
-      <c r="J2" s="23" t="b">
-        <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
-        <v>1</v>
-      </c>
-      <c r="K2" s="23" t="b">
-        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!E2)</f>
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1073,74 +1005,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="D1:D2 F2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.46"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>4</v>
-      </c>
       <c r="D2" s="4" t="n">
-        <v>150</v>
-      </c>
-      <c r="E2" s="17" t="n">
-        <v>45642</v>
-      </c>
-      <c r="F2" s="17" t="n">
-        <f aca="false">E2+20</f>
-        <v>45662</v>
-      </c>
-      <c r="G2" s="4" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H2" s="23" t="b">
-        <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
-        <v>1</v>
-      </c>
-      <c r="I2" s="23" t="b">
-        <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!E2)</f>
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -1159,16 +1058,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="D1:D2 H1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,41 +1075,11 @@
         <v>62</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>150</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="G2" s="4" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -1230,59 +1099,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D2 A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="n">
-        <v>8</v>
-      </c>
       <c r="C2" s="4" t="n">
-        <v>4</v>
+        <v>0.9</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>150</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="4" t="n">
-        <v>4</v>
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -1301,79 +1152,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D1:D2 A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.91"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="n">
+      <c r="D2" s="4" t="n">
         <v>4</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>150</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J2" s="4" t="n">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -1392,46 +1205,101 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.91"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="D1:D2 E2"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>150</v>
-      </c>
-      <c r="E2" s="4" t="n">
         <v>0.6</v>
       </c>
     </row>
@@ -1454,7 +1322,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D2 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1706,7 +1574,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="D1:D2 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1862,7 +1730,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D1:D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2325,7 +2193,7 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D2 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2784,7 +2652,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D2 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2981,7 +2849,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="D1:D2 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3113,7 +2981,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="1" sqref="D1:D2 F6"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3333,7 +3201,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D1:D2 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add AMPL model with overflow
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
+++ b/ampl-data-input-excel/01-no-bounds/01-no-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">Solver</t>
   </si>
   <si>
-    <t xml:space="preserve">With ubday</t>
+    <t xml:space="preserve">AMPL model</t>
   </si>
   <si>
     <t xml:space="preserve">Last day</t>
@@ -214,7 +214,7 @@
     <t xml:space="preserve">scip</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes</t>
+    <t xml:space="preserve">solid</t>
   </si>
   <si>
     <t xml:space="preserve">For all charts</t>
@@ -808,8 +808,8 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -872,7 +872,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>